<commit_message>
create settting to push variable there
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,6 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -455,6 +456,75 @@
       </c>
       <c r="C5">
         <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>source_language</v>
+      </c>
+      <c r="B1" t="str">
+        <v>target_language</v>
+      </c>
+      <c r="C1" t="str">
+        <v>total_tokens</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>You always know after you are two. Two is the beginning of the end.</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Tu toujours</v>
+      </c>
+      <c r="C2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>This was all that passed between them on the subject, but henceforth Wendy knew that she must grow up.</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Cela était</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>They soon know that they will grow up, and the way Wendy knew was this.</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Ils bientôt</v>
+      </c>
+      <c r="C4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>All children, except one, grow up.</v>
+      </c>
+      <c r="B5" t="str">
+        <v>en deserve the opportunity to learn and grow in a safe and supportive environment.</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>